<commit_message>
Added new reports other teams
</commit_message>
<xml_diff>
--- a/Project_Progress.xlsx
+++ b/Project_Progress.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winsen\Documents\GitHub\boekhouding-annemariee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23EF8202-9595-4F91-80FE-6B1ED2ACEF24}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7DD2E7-9D8F-4E28-86F7-15B054018F2C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$41</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Task 3</t>
   </si>
@@ -121,9 +122,6 @@
     <t>Phase 1: Define and set-up project</t>
   </si>
   <si>
-    <t>Define project</t>
-  </si>
-  <si>
     <t>Team</t>
   </si>
   <si>
@@ -148,9 +146,6 @@
     <t>Create project space: GitHub</t>
   </si>
   <si>
-    <t>Analyse potential algorithms</t>
-  </si>
-  <si>
     <t>Tijn</t>
   </si>
   <si>
@@ -169,13 +164,49 @@
     <t>Deadline</t>
   </si>
   <si>
-    <t>Worked on shit</t>
-  </si>
-  <si>
     <t>Project duration</t>
   </si>
   <si>
     <t>Phase 4 Implementing models</t>
+  </si>
+  <si>
+    <t>Discuss project and main objectives</t>
+  </si>
+  <si>
+    <t>Research methods of analysing data</t>
+  </si>
+  <si>
+    <t>Determine how to handle missing data</t>
+  </si>
+  <si>
+    <t>Analyse how to handle data</t>
+  </si>
+  <si>
+    <t>Convert to csv to hdf to speed up processing</t>
+  </si>
+  <si>
+    <t>Initialise central database and align each computer. Create a well-structured folder structure</t>
+  </si>
+  <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>Discuss and set-up project</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>As the base is set-up, find 2 report each, describing how to handle data and which algos are used</t>
   </si>
 </sst>
 </file>
@@ -576,7 +607,7 @@
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -840,6 +871,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1340,11 +1373,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL44"/>
+  <dimension ref="A1:BM44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,9 +1394,9 @@
     <col min="69" max="70" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:65" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1372,14 +1405,14 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:65" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:65" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -1389,7 +1422,7 @@
       </c>
       <c r="F3" s="90"/>
     </row>
-    <row r="4" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1477,7 +1510,7 @@
       <c r="BK4" s="87"/>
       <c r="BL4" s="88"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="G5" s="6"/>
       <c r="I5" s="13">
@@ -1705,7 +1738,7 @@
         <v>43275.35</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:65" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19"/>
       <c r="B6" s="10" t="s">
         <v>13</v>
@@ -1951,10 +1984,10 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19"/>
       <c r="B7" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="22"/>
@@ -2026,7 +2059,7 @@
       <c r="BK7" s="81"/>
       <c r="BL7" s="81"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19"/>
       <c r="B8" s="26" t="s">
         <v>16</v>
@@ -2097,16 +2130,16 @@
       <c r="BK8" s="81"/>
       <c r="BL8" s="81"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" s="33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="34">
         <v>43230</v>
@@ -2176,13 +2209,13 @@
       <c r="BK9" s="81"/>
       <c r="BL9" s="81"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
       <c r="B10" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="33">
         <v>1</v>
@@ -2255,16 +2288,16 @@
       <c r="BK10" s="81"/>
       <c r="BL10" s="81"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="34">
         <v>43230</v>
@@ -2333,14 +2366,17 @@
       <c r="BJ11" s="81"/>
       <c r="BK11" s="81"/>
       <c r="BL11" s="81"/>
+      <c r="BM11" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="32" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>21</v>
       </c>
       <c r="D12" s="33">
         <v>1</v>
@@ -2413,16 +2449,16 @@
       <c r="BK12" s="81"/>
       <c r="BL12" s="81"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="31" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="33">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E13" s="34">
         <v>43230</v>
@@ -2491,11 +2527,14 @@
       <c r="BJ13" s="81"/>
       <c r="BK13" s="81"/>
       <c r="BL13" s="81"/>
+      <c r="BM13" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="37"/>
@@ -2563,25 +2602,25 @@
       <c r="BK14" s="81"/>
       <c r="BL14" s="81"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="42">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E15" s="43">
-        <v>43235</v>
+        <v>43230</v>
       </c>
       <c r="F15" s="44">
-        <v>43235</v>
+        <v>43231</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="81"/>
       <c r="J15" s="81"/>
@@ -2640,20 +2679,20 @@
       <c r="BK15" s="81"/>
       <c r="BL15" s="81"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="40" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="42">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E16" s="43">
-        <v>43230</v>
+        <v>43231</v>
       </c>
       <c r="F16" s="44">
-        <v>43230</v>
+        <v>43231</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25">
@@ -2945,7 +2984,7 @@
     <row r="20" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="46"/>
       <c r="D20" s="47"/>
@@ -3391,7 +3430,7 @@
     <row r="26" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19"/>
       <c r="B26" s="55" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="57"/>
@@ -3837,7 +3876,7 @@
     <row r="32" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="19"/>
       <c r="B32" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="66"/>
       <c r="D32" s="67"/>
@@ -4208,7 +4247,7 @@
     <row r="37" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="19"/>
       <c r="B37" s="70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C37" s="71"/>
       <c r="D37" s="72">
@@ -4653,4 +4692,51 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DF15D9-C6C8-4F91-96CC-110D40489FC5}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="92" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="91">
+        <v>43230</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the progress report
</commit_message>
<xml_diff>
--- a/Project_Progress.xlsx
+++ b/Project_Progress.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winsen\Documents\GitHub\boekhouding-annemariee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7DD2E7-9D8F-4E28-86F7-15B054018F2C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2F4126-427B-46C1-AED2-F6C6259097DF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$42</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!$D1</definedName>
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
-    <definedName name="today" localSheetId="0">ProjectSchedule!$F$43</definedName>
+    <definedName name="today" localSheetId="0">ProjectSchedule!$F$44</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Task 3</t>
   </si>
@@ -207,6 +207,30 @@
   </si>
   <si>
     <t>As the base is set-up, find 2 report each, describing how to handle data and which algos are used</t>
+  </si>
+  <si>
+    <t>Meet to discuss findings</t>
+  </si>
+  <si>
+    <t>11 May - 13 May</t>
+  </si>
+  <si>
+    <t>Research methods how to solve</t>
+  </si>
+  <si>
+    <t>Discuss methods how to solve</t>
+  </si>
+  <si>
+    <t>Check distribution of independent variables per book, click &amp; non-clicked and fill data based on these distrbutions</t>
+  </si>
+  <si>
+    <t>Remove year, min and sec</t>
+  </si>
+  <si>
+    <t>In paper of Xu, features are removed based on their correlation. However, which one to remove? As this is not named, we could include PCA/CFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to convert prices from full stay to daily? </t>
   </si>
 </sst>
 </file>
@@ -607,7 +631,7 @@
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -856,6 +880,7 @@
     <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -871,8 +896,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1373,11 +1405,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BM44"/>
+  <dimension ref="A1:BM45"/>
   <sheetViews>
     <sheetView showGridLines="0" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1417,10 +1449,10 @@
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="89">
+      <c r="E3" s="90">
         <v>43230</v>
       </c>
-      <c r="F3" s="90"/>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:65" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="6" t="s">
@@ -1429,86 +1461,86 @@
       <c r="E4" s="7">
         <v>0.05</v>
       </c>
-      <c r="I4" s="86">
+      <c r="I4" s="87">
         <f>I5</f>
         <v>43220.35</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="86">
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="87">
         <f>P5</f>
         <v>43227.35</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="86">
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="87">
         <f>W5</f>
         <v>43234.35</v>
       </c>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="86">
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="87">
         <f>AD5</f>
         <v>43241.35</v>
       </c>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="86">
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89"/>
+      <c r="AK4" s="87">
         <f>AK5</f>
         <v>43248.35</v>
       </c>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="86">
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="88"/>
+      <c r="AP4" s="88"/>
+      <c r="AQ4" s="89"/>
+      <c r="AR4" s="87">
         <f>AR5</f>
         <v>43255.35</v>
       </c>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="86">
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="88"/>
+      <c r="AX4" s="89"/>
+      <c r="AY4" s="87">
         <f>AY5</f>
         <v>43262.35</v>
       </c>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="86">
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="88"/>
+      <c r="BE4" s="89"/>
+      <c r="BF4" s="87">
         <f>BF5</f>
         <v>43269.35</v>
       </c>
-      <c r="BG4" s="87"/>
-      <c r="BH4" s="87"/>
-      <c r="BI4" s="87"/>
-      <c r="BJ4" s="87"/>
-      <c r="BK4" s="87"/>
-      <c r="BL4" s="88"/>
+      <c r="BG4" s="88"/>
+      <c r="BH4" s="88"/>
+      <c r="BI4" s="88"/>
+      <c r="BJ4" s="88"/>
+      <c r="BK4" s="88"/>
+      <c r="BL4" s="89"/>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
@@ -1999,7 +2031,7 @@
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25">
-        <f t="shared" ref="H7:H41" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H7:H42" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>18</v>
       </c>
       <c r="I7" s="81"/>
@@ -2609,18 +2641,18 @@
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="43">
         <v>43230</v>
       </c>
       <c r="F15" s="44">
-        <v>43231</v>
+        <v>43233</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I15" s="81"/>
       <c r="J15" s="81"/>
@@ -2682,23 +2714,20 @@
     <row r="16" spans="1:65" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="40" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="42">
-        <v>0</v>
-      </c>
-      <c r="E16" s="43">
-        <v>43231</v>
+        <v>1</v>
+      </c>
+      <c r="E16" s="44">
+        <v>43234</v>
       </c>
       <c r="F16" s="44">
-        <v>43231</v>
+        <v>43234</v>
       </c>
       <c r="G16" s="25"/>
-      <c r="H16" s="25">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="H16" s="25"/>
       <c r="I16" s="81"/>
       <c r="J16" s="81"/>
       <c r="K16" s="81"/>
@@ -2711,8 +2740,8 @@
       <c r="R16" s="81"/>
       <c r="S16" s="81"/>
       <c r="T16" s="81"/>
-      <c r="U16" s="82"/>
-      <c r="V16" s="82"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="81"/>
       <c r="W16" s="81"/>
       <c r="X16" s="81"/>
       <c r="Y16" s="81"/>
@@ -2759,15 +2788,17 @@
     <row r="17" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42">
         <v>0</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
       <c r="E17" s="43">
-        <v>43230</v>
+        <v>43231</v>
       </c>
       <c r="F17" s="44">
-        <v>43230</v>
+        <v>43231</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25">
@@ -2786,8 +2817,8 @@
       <c r="R17" s="81"/>
       <c r="S17" s="81"/>
       <c r="T17" s="81"/>
-      <c r="U17" s="81"/>
-      <c r="V17" s="81"/>
+      <c r="U17" s="82"/>
+      <c r="V17" s="82"/>
       <c r="W17" s="81"/>
       <c r="X17" s="81"/>
       <c r="Y17" s="81"/>
@@ -2834,7 +2865,7 @@
     <row r="18" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="42"/>
@@ -2865,7 +2896,7 @@
       <c r="V18" s="81"/>
       <c r="W18" s="81"/>
       <c r="X18" s="81"/>
-      <c r="Y18" s="82"/>
+      <c r="Y18" s="81"/>
       <c r="Z18" s="81"/>
       <c r="AA18" s="81"/>
       <c r="AB18" s="81"/>
@@ -2909,7 +2940,7 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="42"/>
@@ -2940,7 +2971,7 @@
       <c r="V19" s="81"/>
       <c r="W19" s="81"/>
       <c r="X19" s="81"/>
-      <c r="Y19" s="81"/>
+      <c r="Y19" s="82"/>
       <c r="Z19" s="81"/>
       <c r="AA19" s="81"/>
       <c r="AB19" s="81"/>
@@ -2983,17 +3014,21 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
-      <c r="B20" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="49"/>
+      <c r="B20" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43">
+        <v>43230</v>
+      </c>
+      <c r="F20" s="44">
+        <v>43230</v>
+      </c>
       <c r="G20" s="25"/>
-      <c r="H20" s="25" t="str">
+      <c r="H20" s="25">
         <f t="shared" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I20" s="81"/>
       <c r="J20" s="81"/>
@@ -3054,21 +3089,17 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
-      <c r="B21" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53">
-        <v>43230</v>
-      </c>
-      <c r="F21" s="54">
-        <v>43230</v>
-      </c>
+      <c r="B21" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="49"/>
       <c r="G21" s="25"/>
-      <c r="H21" s="25">
+      <c r="H21" s="25" t="str">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I21" s="81"/>
       <c r="J21" s="81"/>
@@ -3130,7 +3161,7 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19"/>
       <c r="B22" s="50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
@@ -3205,7 +3236,7 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
       <c r="B23" s="50" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C23" s="51"/>
       <c r="D23" s="52"/>
@@ -3280,7 +3311,7 @@
     <row r="24" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19"/>
       <c r="B24" s="50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
@@ -3355,7 +3386,7 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19"/>
       <c r="B25" s="50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
@@ -3429,17 +3460,21 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19"/>
-      <c r="B26" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="59"/>
+      <c r="B26" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53">
+        <v>43230</v>
+      </c>
+      <c r="F26" s="54">
+        <v>43230</v>
+      </c>
       <c r="G26" s="25"/>
-      <c r="H26" s="25" t="str">
+      <c r="H26" s="25">
         <f t="shared" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I26" s="81"/>
       <c r="J26" s="81"/>
@@ -3500,21 +3535,17 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="19"/>
-      <c r="B27" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="63">
-        <v>43230</v>
-      </c>
-      <c r="F27" s="64">
-        <v>43230</v>
-      </c>
+      <c r="B27" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
       <c r="G27" s="25"/>
-      <c r="H27" s="25">
+      <c r="H27" s="25" t="str">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I27" s="81"/>
       <c r="J27" s="81"/>
@@ -3576,7 +3607,7 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="19"/>
       <c r="B28" s="60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="61"/>
       <c r="D28" s="62"/>
@@ -3651,7 +3682,7 @@
     <row r="29" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="19"/>
       <c r="B29" s="60" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C29" s="61"/>
       <c r="D29" s="62"/>
@@ -3726,7 +3757,7 @@
     <row r="30" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="19"/>
       <c r="B30" s="60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="61"/>
       <c r="D30" s="62"/>
@@ -3801,7 +3832,7 @@
     <row r="31" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="19"/>
       <c r="B31" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="61"/>
       <c r="D31" s="62"/>
@@ -3875,17 +3906,21 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="19"/>
-      <c r="B32" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="69"/>
+      <c r="B32" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63">
+        <v>43230</v>
+      </c>
+      <c r="F32" s="64">
+        <v>43230</v>
+      </c>
       <c r="G32" s="25"/>
-      <c r="H32" s="25" t="str">
+      <c r="H32" s="25">
         <f t="shared" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I32" s="81"/>
       <c r="J32" s="81"/>
@@ -3946,21 +3981,17 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="19"/>
-      <c r="B33" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="73">
-        <v>43230</v>
-      </c>
-      <c r="F33" s="74">
-        <v>43230</v>
-      </c>
+      <c r="B33" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="66"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="69"/>
       <c r="G33" s="25"/>
-      <c r="H33" s="25">
+      <c r="H33" s="25" t="str">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I33" s="81"/>
       <c r="J33" s="81"/>
@@ -4022,7 +4053,7 @@
     <row r="34" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="19"/>
       <c r="B34" s="70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" s="71"/>
       <c r="D34" s="72"/>
@@ -4097,7 +4128,7 @@
     <row r="35" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19"/>
       <c r="B35" s="70" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C35" s="71"/>
       <c r="D35" s="72"/>
@@ -4172,7 +4203,7 @@
     <row r="36" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="19"/>
       <c r="B36" s="70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="71"/>
       <c r="D36" s="72"/>
@@ -4247,22 +4278,20 @@
     <row r="37" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="19"/>
       <c r="B37" s="70" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C37" s="71"/>
-      <c r="D37" s="72">
-        <v>0.05</v>
-      </c>
+      <c r="D37" s="72"/>
       <c r="E37" s="73">
         <v>43230</v>
       </c>
       <c r="F37" s="74">
-        <v>43247</v>
+        <v>43230</v>
       </c>
       <c r="G37" s="25"/>
       <c r="H37" s="25">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="I37" s="81"/>
       <c r="J37" s="81"/>
@@ -4323,15 +4352,23 @@
     </row>
     <row r="38" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="24"/>
+      <c r="B38" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="71"/>
+      <c r="D38" s="72">
+        <v>0.05</v>
+      </c>
+      <c r="E38" s="73">
+        <v>43230</v>
+      </c>
+      <c r="F38" s="74">
+        <v>43247</v>
+      </c>
       <c r="G38" s="25"/>
-      <c r="H38" s="25" t="str">
+      <c r="H38" s="25">
         <f t="shared" si="6"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="I38" s="81"/>
       <c r="J38" s="81"/>
@@ -4530,93 +4567,162 @@
     </row>
     <row r="41" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="19"/>
-      <c r="B41" s="75" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="80"/>
-      <c r="H41" s="80" t="str">
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I41" s="83"/>
-      <c r="J41" s="83"/>
-      <c r="K41" s="83"/>
-      <c r="L41" s="83"/>
-      <c r="M41" s="83"/>
-      <c r="N41" s="83"/>
-      <c r="O41" s="83"/>
-      <c r="P41" s="83"/>
-      <c r="Q41" s="83"/>
-      <c r="R41" s="83"/>
-      <c r="S41" s="83"/>
-      <c r="T41" s="83"/>
-      <c r="U41" s="83"/>
-      <c r="V41" s="83"/>
-      <c r="W41" s="83"/>
-      <c r="X41" s="83"/>
-      <c r="Y41" s="83"/>
-      <c r="Z41" s="83"/>
-      <c r="AA41" s="83"/>
-      <c r="AB41" s="83"/>
-      <c r="AC41" s="83"/>
-      <c r="AD41" s="83"/>
-      <c r="AE41" s="83"/>
-      <c r="AF41" s="83"/>
-      <c r="AG41" s="83"/>
-      <c r="AH41" s="83"/>
-      <c r="AI41" s="83"/>
-      <c r="AJ41" s="83"/>
-      <c r="AK41" s="83"/>
-      <c r="AL41" s="83"/>
-      <c r="AM41" s="83"/>
-      <c r="AN41" s="83"/>
-      <c r="AO41" s="83"/>
-      <c r="AP41" s="83"/>
-      <c r="AQ41" s="83"/>
-      <c r="AR41" s="83"/>
-      <c r="AS41" s="83"/>
-      <c r="AT41" s="83"/>
-      <c r="AU41" s="83"/>
-      <c r="AV41" s="83"/>
-      <c r="AW41" s="83"/>
-      <c r="AX41" s="83"/>
-      <c r="AY41" s="83"/>
-      <c r="AZ41" s="83"/>
-      <c r="BA41" s="83"/>
-      <c r="BB41" s="83"/>
-      <c r="BC41" s="83"/>
-      <c r="BD41" s="83"/>
-      <c r="BE41" s="83"/>
-      <c r="BF41" s="83"/>
-      <c r="BG41" s="83"/>
-      <c r="BH41" s="83"/>
-      <c r="BI41" s="83"/>
-      <c r="BJ41" s="83"/>
-      <c r="BK41" s="83"/>
-      <c r="BL41" s="83"/>
-    </row>
-    <row r="42" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="81"/>
+      <c r="L41" s="81"/>
+      <c r="M41" s="81"/>
+      <c r="N41" s="81"/>
+      <c r="O41" s="81"/>
+      <c r="P41" s="81"/>
+      <c r="Q41" s="81"/>
+      <c r="R41" s="81"/>
+      <c r="S41" s="81"/>
+      <c r="T41" s="81"/>
+      <c r="U41" s="81"/>
+      <c r="V41" s="81"/>
+      <c r="W41" s="81"/>
+      <c r="X41" s="81"/>
+      <c r="Y41" s="81"/>
+      <c r="Z41" s="81"/>
+      <c r="AA41" s="81"/>
+      <c r="AB41" s="81"/>
+      <c r="AC41" s="81"/>
+      <c r="AD41" s="81"/>
+      <c r="AE41" s="81"/>
+      <c r="AF41" s="81"/>
+      <c r="AG41" s="81"/>
+      <c r="AH41" s="81"/>
+      <c r="AI41" s="81"/>
+      <c r="AJ41" s="81"/>
+      <c r="AK41" s="81"/>
+      <c r="AL41" s="81"/>
+      <c r="AM41" s="81"/>
+      <c r="AN41" s="81"/>
+      <c r="AO41" s="81"/>
+      <c r="AP41" s="81"/>
+      <c r="AQ41" s="81"/>
+      <c r="AR41" s="81"/>
+      <c r="AS41" s="81"/>
+      <c r="AT41" s="81"/>
+      <c r="AU41" s="81"/>
+      <c r="AV41" s="81"/>
+      <c r="AW41" s="81"/>
+      <c r="AX41" s="81"/>
+      <c r="AY41" s="81"/>
+      <c r="AZ41" s="81"/>
+      <c r="BA41" s="81"/>
+      <c r="BB41" s="81"/>
+      <c r="BC41" s="81"/>
+      <c r="BD41" s="81"/>
+      <c r="BE41" s="81"/>
+      <c r="BF41" s="81"/>
+      <c r="BG41" s="81"/>
+      <c r="BH41" s="81"/>
+      <c r="BI41" s="81"/>
+      <c r="BJ41" s="81"/>
+      <c r="BK41" s="81"/>
+      <c r="BL41" s="81"/>
+    </row>
+    <row r="42" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="19"/>
+      <c r="B42" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="76"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="79"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="80" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I42" s="83"/>
+      <c r="J42" s="83"/>
+      <c r="K42" s="83"/>
+      <c r="L42" s="83"/>
+      <c r="M42" s="83"/>
+      <c r="N42" s="83"/>
+      <c r="O42" s="83"/>
+      <c r="P42" s="83"/>
+      <c r="Q42" s="83"/>
+      <c r="R42" s="83"/>
+      <c r="S42" s="83"/>
+      <c r="T42" s="83"/>
+      <c r="U42" s="83"/>
+      <c r="V42" s="83"/>
+      <c r="W42" s="83"/>
+      <c r="X42" s="83"/>
+      <c r="Y42" s="83"/>
+      <c r="Z42" s="83"/>
+      <c r="AA42" s="83"/>
+      <c r="AB42" s="83"/>
+      <c r="AC42" s="83"/>
+      <c r="AD42" s="83"/>
+      <c r="AE42" s="83"/>
+      <c r="AF42" s="83"/>
+      <c r="AG42" s="83"/>
+      <c r="AH42" s="83"/>
+      <c r="AI42" s="83"/>
+      <c r="AJ42" s="83"/>
+      <c r="AK42" s="83"/>
+      <c r="AL42" s="83"/>
+      <c r="AM42" s="83"/>
+      <c r="AN42" s="83"/>
+      <c r="AO42" s="83"/>
+      <c r="AP42" s="83"/>
+      <c r="AQ42" s="83"/>
+      <c r="AR42" s="83"/>
+      <c r="AS42" s="83"/>
+      <c r="AT42" s="83"/>
+      <c r="AU42" s="83"/>
+      <c r="AV42" s="83"/>
+      <c r="AW42" s="83"/>
+      <c r="AX42" s="83"/>
+      <c r="AY42" s="83"/>
+      <c r="AZ42" s="83"/>
+      <c r="BA42" s="83"/>
+      <c r="BB42" s="83"/>
+      <c r="BC42" s="83"/>
+      <c r="BD42" s="83"/>
+      <c r="BE42" s="83"/>
+      <c r="BF42" s="83"/>
+      <c r="BG42" s="83"/>
+      <c r="BH42" s="83"/>
+      <c r="BI42" s="83"/>
+      <c r="BJ42" s="83"/>
+      <c r="BK42" s="83"/>
+      <c r="BL42" s="83"/>
     </row>
     <row r="43" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="B43" s="17" t="s">
+      <c r="A43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="F43" s="85">
+      <c r="C44" s="17"/>
+      <c r="F44" s="85">
         <v>43113</v>
       </c>
     </row>
-    <row r="44" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="B44" s="18" t="s">
+    <row r="45" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="B45" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="18"/>
+      <c r="C45" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4630,7 +4736,7 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D41">
+  <conditionalFormatting sqref="D7:D42">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4644,7 +4750,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL41">
+  <conditionalFormatting sqref="I7:BL42">
     <cfRule type="expression" dxfId="2" priority="25">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4652,9 +4758,9 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL41">
+  <conditionalFormatting sqref="I5:BL42">
     <cfRule type="expression" dxfId="0" priority="27">
-      <formula>AND($F$43&gt;=I$5,$F$43&lt;J$5)</formula>
+      <formula>AND($F$44&gt;=I$5,$F$44&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4663,8 +4769,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B44" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B43" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B45" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B44" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId3"/>
@@ -4686,7 +4792,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D41</xm:sqref>
+          <xm:sqref>D7:D42</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4696,15 +4802,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DF15D9-C6C8-4F91-96CC-110D40489FC5}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="94" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="80.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4712,18 +4819,18 @@
       <c r="A1" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="86" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="91">
+      <c r="A2" s="93">
         <v>43230</v>
       </c>
       <c r="B2" t="s">
@@ -4734,6 +4841,40 @@
       </c>
       <c r="D2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="94" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="93">
+        <v>43234</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>